<commit_message>
Renamed sheets and a couple columns for consistency
</commit_message>
<xml_diff>
--- a/data/raw/day_ahead_price_profile.xlsx
+++ b/data/raw/day_ahead_price_profile.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3897AE50-B51D-4176-BA54-C547E9CD482A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77613A5-EDEB-4284-8C6B-1587914F53EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1370" windowWidth="19200" windowHeight="8830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DA_Price" sheetId="1" r:id="rId1"/>
+    <sheet name="Price" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -361,7 +361,7 @@
   <dimension ref="A1:Z61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>